<commit_message>
Correcciones al 20 de Junio
Se van trabajando 17 correcciones hasta el momento
</commit_message>
<xml_diff>
--- a/correcciones.xlsx
+++ b/correcciones.xlsx
@@ -158,10 +158,10 @@
     <t>54-59</t>
   </si>
   <si>
-    <t>19, 25, 28, 29, 52, 80</t>
-  </si>
-  <si>
-    <t xml:space="preserve">19, 21, 25, 27, 29, </t>
+    <t>19, 21, 25, 27, 28, 29, 52, 80</t>
+  </si>
+  <si>
+    <t>A lo largo del documento se cambio 'sistema' por 'software' donde se necesitaba</t>
   </si>
 </sst>
 </file>
@@ -275,7 +275,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="4"/>
@@ -317,6 +317,7 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="16" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="16" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -634,7 +635,7 @@
   <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -923,7 +924,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="38" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="38" x14ac:dyDescent="0.25">
       <c r="A17" s="12"/>
       <c r="B17" s="4" t="s">
         <v>16</v>
@@ -937,7 +938,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="38" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" ht="38" x14ac:dyDescent="0.25">
       <c r="A18" s="12"/>
       <c r="B18" s="4" t="s">
         <v>17</v>
@@ -955,7 +956,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="57" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="57" x14ac:dyDescent="0.25">
       <c r="A19" s="12"/>
       <c r="B19" s="4" t="s">
         <v>18</v>
@@ -969,7 +970,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A20" s="12"/>
       <c r="B20" s="5" t="s">
         <v>19</v>
@@ -987,7 +988,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A21" s="12"/>
       <c r="B21" s="5" t="s">
         <v>20</v>
@@ -1005,7 +1006,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="38" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" ht="57" x14ac:dyDescent="0.25">
       <c r="A22" s="12"/>
       <c r="B22" s="4" t="s">
         <v>21</v>
@@ -1016,12 +1017,17 @@
       <c r="D22" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="E22" s="5"/>
+      <c r="E22" s="17">
+        <v>43269</v>
+      </c>
       <c r="F22" s="18">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" ht="38" x14ac:dyDescent="0.25">
+      <c r="G22" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="38" x14ac:dyDescent="0.25">
       <c r="A23" s="13" t="s">
         <v>25</v>
       </c>
@@ -1031,15 +1037,17 @@
       <c r="C23" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="D23" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="E23" s="8"/>
-      <c r="F23" s="18">
+      <c r="D23" s="8">
+        <v>13</v>
+      </c>
+      <c r="E23" s="19">
+        <v>43269</v>
+      </c>
+      <c r="F23" s="16">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:6" ht="19" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A24" s="13"/>
       <c r="B24" s="8" t="s">
         <v>24</v>

</xml_diff>

<commit_message>
Correcciones al 21 de Junio
Faltan 3 correcciones, de las cuales 2 se encuentran en 60%
</commit_message>
<xml_diff>
--- a/correcciones.xlsx
+++ b/correcciones.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="56">
   <si>
     <t>Estudios posteriores: definirlos más específicamente.  Enfocarlos en los hallazgos del estudio.</t>
   </si>
@@ -162,6 +162,39 @@
   </si>
   <si>
     <t>A lo largo del documento se cambio 'sistema' por 'software' donde se necesitaba</t>
+  </si>
+  <si>
+    <t>71-74</t>
+  </si>
+  <si>
+    <t>Se añadio explicaciones detalladas a la creación de cada pantalla</t>
+  </si>
+  <si>
+    <t>82-85</t>
+  </si>
+  <si>
+    <t>Se explico a detalle sistemas analogos presentados en latinoamerica para recoleccion de reclamos o peticiones en salud.</t>
+  </si>
+  <si>
+    <t>Marco Teorico / Discusión</t>
+  </si>
+  <si>
+    <t>24-25 / 82-85</t>
+  </si>
+  <si>
+    <t>Marco Teorico: Se agrego parrafo sobre busqueda bibliografica de sistemas similares. Discusión: Se agrego en extensión explicación sobre la funcionalidad de dos sistemas simialres presentados en latinoamerica.</t>
+  </si>
+  <si>
+    <t>Se agrego un parrafo sobre el uso de UCD en otros sistemas inofmraticos clinicos que utilizaran de forma trascendental la opinion de usuarios para reforzar lo encontrado</t>
+  </si>
+  <si>
+    <t>17-18</t>
+  </si>
+  <si>
+    <t>Se agrego un parrafo de explicación sobre las variables cualitativas a utilizarse para las pruebas de usuario para ser más explicito</t>
+  </si>
+  <si>
+    <t>Se restructuro toda la parte de resultados para la fase exploratoria</t>
   </si>
 </sst>
 </file>
@@ -237,7 +270,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -271,11 +304,20 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="4"/>
@@ -318,6 +360,13 @@
     <xf numFmtId="16" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="16" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -634,14 +683,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="79" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="42.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="19" x14ac:dyDescent="0.25">
@@ -751,10 +801,17 @@
       <c r="C6" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6">
+      <c r="D6" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="E6" s="17">
+        <v>43272</v>
+      </c>
+      <c r="F6" s="16">
         <v>5</v>
+      </c>
+      <c r="G6" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="57" x14ac:dyDescent="0.25">
@@ -796,18 +853,25 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="38" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="114" x14ac:dyDescent="0.25">
       <c r="A9" s="12"/>
       <c r="B9" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="18">
+      <c r="C9" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E9" s="17">
+        <v>43271</v>
+      </c>
+      <c r="F9" s="16">
         <v>8</v>
+      </c>
+      <c r="G9" s="20" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="38" x14ac:dyDescent="0.25">
@@ -873,9 +937,14 @@
         <v>35</v>
       </c>
       <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13">
+      <c r="E13" s="17">
+        <v>43272</v>
+      </c>
+      <c r="F13" s="22">
         <v>12</v>
+      </c>
+      <c r="G13" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="38" x14ac:dyDescent="0.25">
@@ -904,10 +973,17 @@
       <c r="C15" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="18">
+      <c r="D15" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="E15" s="17">
+        <v>43271</v>
+      </c>
+      <c r="F15" s="16">
         <v>14</v>
+      </c>
+      <c r="G15" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="19" x14ac:dyDescent="0.25">
@@ -920,7 +996,7 @@
       </c>
       <c r="D16" s="5"/>
       <c r="E16" s="5"/>
-      <c r="F16">
+      <c r="F16" s="18">
         <v>15</v>
       </c>
     </row>
@@ -934,7 +1010,7 @@
       </c>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
-      <c r="F17">
+      <c r="F17" s="18">
         <v>16</v>
       </c>
     </row>
@@ -956,7 +1032,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="57" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" ht="65" x14ac:dyDescent="0.25">
       <c r="A19" s="12"/>
       <c r="B19" s="4" t="s">
         <v>18</v>
@@ -964,10 +1040,17 @@
       <c r="C19" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19">
+      <c r="D19" s="5">
+        <v>86</v>
+      </c>
+      <c r="E19" s="17">
+        <v>43271</v>
+      </c>
+      <c r="F19" s="16">
         <v>18</v>
+      </c>
+      <c r="G19" s="21" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="19" x14ac:dyDescent="0.25">
@@ -1020,7 +1103,7 @@
       <c r="E22" s="17">
         <v>43269</v>
       </c>
-      <c r="F22" s="18">
+      <c r="F22" s="16">
         <v>21</v>
       </c>
       <c r="G22" t="s">
@@ -1053,10 +1136,17 @@
         <v>24</v>
       </c>
       <c r="C24" s="8"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="8"/>
-      <c r="F24" s="18">
+      <c r="D24" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="E24" s="19">
+        <v>43271</v>
+      </c>
+      <c r="F24" s="16">
         <v>23</v>
+      </c>
+      <c r="G24" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="33" spans="4:4" x14ac:dyDescent="0.2">

</xml_diff>